<commit_message>
Custom Routing Added along with Unit Tests
</commit_message>
<xml_diff>
--- a/THSurveys/ModelsAndDocuments/Documents/Design/RoutingTable.xlsx
+++ b/THSurveys/ModelsAndDocuments/Documents/Design/RoutingTable.xlsx
@@ -16,8 +16,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tim Harrison</author>
+  </authors>
+  <commentList>
+    <comment ref="L24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tim Harrison:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Inserted a specific route to handle this Url.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="228">
   <si>
     <t>URL</t>
   </si>
@@ -2479,12 +2513,18 @@
   <si>
     <t>Y</t>
   </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>input (approvals)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2596,6 +2636,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="16">
@@ -2800,15 +2853,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2849,6 +2893,15 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -3168,11 +3221,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="53"/>
       <c r="F1" s="9"/>
       <c r="G1" s="10"/>
     </row>
@@ -3335,7 +3388,7 @@
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="26" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -3364,7 +3417,7 @@
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="27" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -3591,7 +3644,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="28" t="s">
         <v>102</v>
       </c>
       <c r="E23" t="s">
@@ -3628,11 +3681,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3649,38 +3702,38 @@
     <col min="12" max="12" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="27" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:12" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>214</v>
       </c>
     </row>
@@ -3691,10 +3744,10 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="50" t="s">
         <v>177</v>
       </c>
       <c r="G2" t="s">
@@ -3709,7 +3762,7 @@
       <c r="J2" t="s">
         <v>207</v>
       </c>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="43" t="s">
         <v>215</v>
       </c>
       <c r="L2" t="s">
@@ -3723,10 +3776,10 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="50" t="s">
         <v>109</v>
       </c>
       <c r="G3" t="s">
@@ -3741,7 +3794,7 @@
       <c r="J3" t="s">
         <v>207</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="43" t="s">
         <v>215</v>
       </c>
       <c r="L3" t="s">
@@ -3755,10 +3808,10 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="50" t="s">
         <v>168</v>
       </c>
       <c r="G4" t="s">
@@ -3767,8 +3820,11 @@
       <c r="H4" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="44" t="s">
+      <c r="K4" s="41" t="s">
         <v>221</v>
+      </c>
+      <c r="L4" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3778,10 +3834,10 @@
       <c r="B5" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="50" t="s">
         <v>169</v>
       </c>
       <c r="G5" t="s">
@@ -3796,8 +3852,11 @@
       <c r="J5" t="s">
         <v>207</v>
       </c>
-      <c r="K5" s="49" t="s">
+      <c r="K5" s="46" t="s">
         <v>218</v>
+      </c>
+      <c r="L5" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -3810,10 +3869,10 @@
       <c r="C6" t="s">
         <v>130</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="50" t="s">
         <v>176</v>
       </c>
       <c r="G6" t="s">
@@ -3828,8 +3887,11 @@
       <c r="J6" t="s">
         <v>209</v>
       </c>
-      <c r="K6" s="51" t="s">
+      <c r="K6" s="48" t="s">
         <v>223</v>
+      </c>
+      <c r="L6" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3842,10 +3904,10 @@
       <c r="C7" t="s">
         <v>134</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="50" t="s">
         <v>178</v>
       </c>
       <c r="G7" t="s">
@@ -3860,8 +3922,11 @@
       <c r="J7" t="s">
         <v>209</v>
       </c>
-      <c r="K7" s="50" t="s">
+      <c r="K7" s="47" t="s">
         <v>216</v>
+      </c>
+      <c r="L7" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3880,7 +3945,7 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="25" t="s">
         <v>183</v>
       </c>
       <c r="G8" t="s">
@@ -3895,8 +3960,11 @@
       <c r="J8" t="s">
         <v>209</v>
       </c>
-      <c r="K8" s="45" t="s">
+      <c r="K8" s="42" t="s">
         <v>217</v>
+      </c>
+      <c r="L8" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3912,7 +3980,7 @@
       <c r="E9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="25" t="s">
         <v>179</v>
       </c>
       <c r="G9" t="s">
@@ -3927,8 +3995,11 @@
       <c r="J9" t="s">
         <v>209</v>
       </c>
-      <c r="K9" s="50" t="s">
+      <c r="K9" s="47" t="s">
         <v>216</v>
+      </c>
+      <c r="L9" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3938,10 +4009,10 @@
       <c r="B10" t="s">
         <v>144</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="50" t="s">
         <v>97</v>
       </c>
       <c r="G10" t="s">
@@ -3956,7 +4027,7 @@
       <c r="J10" t="s">
         <v>207</v>
       </c>
-      <c r="K10" s="46" t="s">
+      <c r="K10" s="43" t="s">
         <v>215</v>
       </c>
       <c r="L10" t="s">
@@ -3970,10 +4041,10 @@
       <c r="B11" t="s">
         <v>145</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="53" t="s">
+      <c r="F11" s="50" t="s">
         <v>98</v>
       </c>
       <c r="G11" t="s">
@@ -3988,7 +4059,7 @@
       <c r="J11" t="s">
         <v>207</v>
       </c>
-      <c r="K11" s="46" t="s">
+      <c r="K11" s="43" t="s">
         <v>215</v>
       </c>
       <c r="L11" t="s">
@@ -3996,243 +4067,249 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="42" t="s">
+      <c r="B12" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="53" t="s">
+      <c r="F12" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="J12" s="38" t="s">
+      <c r="J12" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="K12" s="43" t="s">
+      <c r="K12" s="40" t="s">
         <v>222</v>
       </c>
+      <c r="L12" s="35" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="42" t="s">
+      <c r="B13" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="53" t="s">
+      <c r="F13" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="H13" s="38" t="s">
+      <c r="H13" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="I13" s="38" t="s">
+      <c r="I13" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="J13" s="38" t="s">
+      <c r="J13" s="35" t="s">
         <v>207</v>
       </c>
-      <c r="K13" s="46" t="s">
+      <c r="K13" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="L13" s="38" t="s">
+      <c r="L13" s="35" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="42" t="s">
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="53" t="s">
+      <c r="F14" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="I14" s="38" t="s">
+      <c r="I14" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="J14" s="38" t="s">
+      <c r="J14" s="35" t="s">
         <v>207</v>
       </c>
-      <c r="K14" s="46" t="s">
+      <c r="K14" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="L14" s="38" t="s">
+      <c r="L14" s="35" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="39" t="s">
+      <c r="F15" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="H15" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="I15" s="38" t="s">
+      <c r="I15" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="J15" s="38" t="s">
+      <c r="J15" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="K15" s="48" t="s">
+      <c r="K15" s="45" t="s">
         <v>219</v>
       </c>
+      <c r="L15" s="35" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="C16" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="38" t="s">
+      <c r="C16" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="39" t="s">
+      <c r="F16" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="G16" s="38" t="s">
+      <c r="G16" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="J16" s="38" t="s">
+      <c r="J16" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="K16" s="47" t="s">
+      <c r="K16" s="44" t="s">
         <v>220</v>
       </c>
-      <c r="L16" s="38" t="s">
+      <c r="L16" s="35" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="42" t="s">
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="53" t="s">
+      <c r="F17" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="H17" s="38" t="s">
+      <c r="H17" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="I17" s="38" t="s">
+      <c r="I17" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="J17" s="38" t="s">
+      <c r="J17" s="35" t="s">
         <v>207</v>
       </c>
-      <c r="K17" s="46" t="s">
+      <c r="K17" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="L17" s="38" t="s">
+      <c r="L17" s="35" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="D18" s="38" t="s">
+      <c r="C18" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="D18" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="G18" s="38" t="s">
+      <c r="G18" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="H18" s="38" t="s">
+      <c r="H18" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="I18" s="38" t="s">
+      <c r="I18" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="J18" s="38" t="s">
+      <c r="J18" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="K18" s="48" t="s">
+      <c r="K18" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -4244,12 +4321,12 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>186</v>
       </c>
       <c r="G19" t="s">
@@ -4264,8 +4341,11 @@
       <c r="J19" t="s">
         <v>209</v>
       </c>
-      <c r="K19" s="51" t="s">
+      <c r="K19" s="48" t="s">
         <v>223</v>
+      </c>
+      <c r="L19" s="35" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -4284,7 +4364,7 @@
       <c r="E20" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="25" t="s">
         <v>187</v>
       </c>
       <c r="G20" t="s">
@@ -4299,8 +4379,11 @@
       <c r="J20" t="s">
         <v>209</v>
       </c>
-      <c r="K20" s="52" t="s">
+      <c r="K20" s="49" t="s">
         <v>224</v>
+      </c>
+      <c r="L20" s="35" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -4319,7 +4402,7 @@
       <c r="E21" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="25" t="s">
         <v>173</v>
       </c>
       <c r="G21" t="s">
@@ -4334,8 +4417,11 @@
       <c r="J21" t="s">
         <v>209</v>
       </c>
-      <c r="K21" s="47" t="s">
+      <c r="K21" s="44" t="s">
         <v>220</v>
+      </c>
+      <c r="L21" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -4354,7 +4440,7 @@
       <c r="E22" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="25" t="s">
         <v>172</v>
       </c>
       <c r="G22" t="s">
@@ -4369,82 +4455,91 @@
       <c r="J22" t="s">
         <v>209</v>
       </c>
-      <c r="K22" s="47" t="s">
+      <c r="K22" s="44" t="s">
         <v>220</v>
       </c>
+      <c r="L22" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="53" t="s">
+      <c r="F23" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="G23" s="38" t="s">
+      <c r="G23" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="H23" s="38" t="s">
+      <c r="H23" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="I23" s="38" t="s">
+      <c r="I23" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="J23" s="38" t="s">
+      <c r="J23" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="K23" s="51" t="s">
+      <c r="K23" s="48" t="s">
         <v>223</v>
       </c>
+      <c r="L23" s="35" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D24" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="G24" s="38" t="s">
+      <c r="G24" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="H24" s="38" t="s">
+      <c r="H24" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="I24" s="38" t="s">
+      <c r="I24" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="J24" s="38" t="s">
+      <c r="J24" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="K24" s="47" t="s">
+      <c r="K24" s="44" t="s">
         <v>220</v>
       </c>
+      <c r="L24" s="35" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="23" t="s">
         <v>190</v>
       </c>
     </row>
@@ -4452,47 +4547,47 @@
       <c r="A27" t="s">
         <v>191</v>
       </c>
-      <c r="G27" s="46" t="s">
+      <c r="G27" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="H27" s="49" t="s">
+      <c r="H27" s="46" t="s">
         <v>218</v>
       </c>
-      <c r="I27" s="44" t="s">
+      <c r="I27" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="J27" s="44"/>
+      <c r="J27" s="41"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>192</v>
       </c>
-      <c r="G28" s="47" t="s">
+      <c r="G28" s="44" t="s">
         <v>220</v>
       </c>
-      <c r="H28" s="50" t="s">
+      <c r="H28" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="I28" s="51" t="s">
+      <c r="I28" s="48" t="s">
         <v>223</v>
       </c>
-      <c r="J28" s="51"/>
+      <c r="J28" s="48"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>193</v>
       </c>
-      <c r="G29" s="48" t="s">
+      <c r="G29" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="H29" s="45" t="s">
+      <c r="H29" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="I29" s="52" t="s">
+      <c r="I29" s="49" t="s">
         <v>224</v>
       </c>
-      <c r="J29" s="52"/>
-      <c r="K29" s="43" t="s">
+      <c r="J29" s="49"/>
+      <c r="K29" s="40" t="s">
         <v>222</v>
       </c>
     </row>
@@ -4523,6 +4618,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4536,300 +4632,300 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.28515625" style="37" customWidth="1"/>
+    <col min="1" max="1" width="87.28515625" style="34" customWidth="1"/>
     <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="27" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:2" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="25" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="25" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="25" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+      <c r="A8" s="31"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="25" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="25" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+      <c r="A13" s="31"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="31" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="25" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="31"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="31" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="25" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="32"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="25" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="32" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
+      <c r="A22" s="32"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="32" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="25" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="32" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="25" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="25" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="25" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="25" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
+      <c r="A30" s="32"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="32" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="25" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+      <c r="A33" s="32"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="32" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="25" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
+      <c r="A36" s="32"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="32" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="25" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
+      <c r="A39" s="32"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="32" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="25" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="25" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="B43" s="25" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
+      <c r="A44" s="31"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="31" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="B46" s="28" t="s">
+      <c r="B46" s="25" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
+      <c r="A47" s="31"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
+      <c r="A48" s="32"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+      <c r="A49" s="32"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -4837,16 +4933,16 @@
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="34"/>
+      <c r="A51" s="31"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="34"/>
+      <c r="A52" s="31"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="34"/>
+      <c r="A53" s="31"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
+      <c r="A54" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -4875,26 +4971,26 @@
     <col min="7" max="7" width="101" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="27" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:7" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="24" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simple styling added and all pages linked
Simple style added to all pages, menu added and all pages linked.
</commit_message>
<xml_diff>
--- a/THSurveys/ModelsAndDocuments/Documents/Design/RoutingTable.xlsx
+++ b/THSurveys/ModelsAndDocuments/Documents/Design/RoutingTable.xlsx
@@ -2651,7 +2651,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2740,6 +2740,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -2815,7 +2821,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2902,6 +2908,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -3685,7 +3693,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3869,10 +3877,10 @@
       <c r="C6" t="s">
         <v>130</v>
       </c>
-      <c r="E6" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="50" t="s">
+      <c r="E6" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="55" t="s">
         <v>176</v>
       </c>
       <c r="G6" t="s">

</xml_diff>